<commit_message>
Remove redundant values in base.xlsx
</commit_message>
<xml_diff>
--- a/data/scenarios/base.xlsx
+++ b/data/scenarios/base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilhelmwanecek/dev/exjobb/eitm01-scenarios/data/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF422DB-0181-E74D-A7EC-0021FDD4500F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A505B4A-FDA6-3F4A-99EC-E4DBB630B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="29400" windowHeight="18360" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="141">
   <si>
     <t>f_crop</t>
   </si>
@@ -238,12 +238,6 @@
     <t>sunflower seed meal</t>
   </si>
   <si>
-    <t>palm kern expeller</t>
-  </si>
-  <si>
-    <t>wheat distillers grain, wet</t>
-  </si>
-  <si>
     <t>Minimum roughage shares</t>
   </si>
   <si>
@@ -259,13 +253,7 @@
     <t>cows</t>
   </si>
   <si>
-    <t>soybean protein concentrated</t>
-  </si>
-  <si>
     <t>calves, suckling</t>
-  </si>
-  <si>
-    <t>whey powder</t>
   </si>
   <si>
     <t>bulls</t>
@@ -4800,10 +4788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5035,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>51</v>
       </c>
@@ -5049,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>52</v>
       </c>
@@ -5063,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>53</v>
       </c>
@@ -5077,7 +5065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
         <v>54</v>
       </c>
@@ -5092,7 +5080,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>55</v>
       </c>
@@ -5106,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>56</v>
       </c>
@@ -5120,7 +5108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>57</v>
       </c>
@@ -5134,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>58</v>
       </c>
@@ -5148,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>59</v>
       </c>
@@ -5162,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>60</v>
       </c>
@@ -5176,7 +5164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>61</v>
       </c>
@@ -5190,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>62</v>
       </c>
@@ -5204,7 +5192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>63</v>
       </c>
@@ -5218,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>64</v>
       </c>
@@ -5232,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>65</v>
       </c>
@@ -5246,38 +5234,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="J32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J34" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="J36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E37" t="s">
-        <v>72</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
@@ -5285,19 +5250,16 @@
       <c r="G37">
         <v>0.75</v>
       </c>
-      <c r="J37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
@@ -5305,19 +5267,16 @@
       <c r="G38" s="5">
         <v>0.5</v>
       </c>
-      <c r="J38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
@@ -5325,16 +5284,13 @@
       <c r="G39" s="5">
         <v>0</v>
       </c>
-      <c r="J39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
         <v>8</v>
@@ -5343,18 +5299,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>44</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
@@ -5363,18 +5319,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
         <v>45</v>
@@ -5389,12 +5345,12 @@
         <v>6.6079520088655102</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
         <v>45</v>
@@ -5409,12 +5365,12 @@
         <v>50.052481882315803</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
         <v>45</v>
@@ -5429,12 +5385,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
         <v>45</v>
@@ -5449,12 +5405,12 @@
         <v>37.9858028062012</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D48" t="s">
         <v>45</v>
@@ -5474,7 +5430,7 @@
         <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D49" t="s">
         <v>45</v>
@@ -5491,10 +5447,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
         <v>45</v>
@@ -5511,10 +5467,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
         <v>45</v>
@@ -5531,10 +5487,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
         <v>45</v>
@@ -5551,10 +5507,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D53" t="s">
         <v>45</v>
@@ -5571,10 +5527,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D54" t="s">
         <v>45</v>
@@ -5591,10 +5547,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
         <v>45</v>
@@ -5611,7 +5567,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B56" s="4"/>
     </row>
@@ -5620,13 +5576,13 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F57" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G57" s="5">
         <v>7.84</v>
@@ -5637,13 +5593,13 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E58" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F58" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G58" s="5">
         <v>8.67</v>
@@ -5654,13 +5610,13 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E59" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F59" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G59" s="5">
         <v>5.21</v>
@@ -5671,13 +5627,13 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E60" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F60" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G60" s="5">
         <v>7.54</v>
@@ -5688,13 +5644,13 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F61" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G61" s="5">
         <v>4.47</v>
@@ -5705,13 +5661,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E62" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F62" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G62" s="5">
         <v>4.62</v>
@@ -5722,13 +5678,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E63" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F63" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G63" s="5">
         <v>0.23</v>
@@ -5739,13 +5695,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F64" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G64" s="5">
         <v>19.190000000000001</v>
@@ -5756,13 +5712,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E65" t="s">
         <v>83</v>
       </c>
-      <c r="E65" t="s">
-        <v>87</v>
-      </c>
       <c r="F65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G65" s="5">
         <v>7.49</v>
@@ -5773,13 +5729,13 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>83</v>
+      </c>
+      <c r="F66" t="s">
         <v>84</v>
-      </c>
-      <c r="E66" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" t="s">
-        <v>88</v>
       </c>
       <c r="G66" s="5">
         <v>8.3800000000000008</v>
@@ -5787,16 +5743,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F67" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G67" s="5">
         <v>8.67</v>
@@ -5804,16 +5760,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E68" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F68" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G68" s="5">
         <v>8.01</v>
@@ -5821,16 +5777,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" t="s">
         <v>85</v>
       </c>
-      <c r="B69" t="s">
-        <v>89</v>
-      </c>
       <c r="E69" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G69" s="5">
         <v>6.15</v>
@@ -5838,16 +5794,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E70" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F70" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G70" s="5">
         <v>3.97</v>
@@ -5855,16 +5811,16 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E71" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F71" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G71" s="5">
         <v>5.7</v>
@@ -5872,16 +5828,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E72" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G72" s="5">
         <v>5.84</v>
@@ -5889,16 +5845,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E73" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F73" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G73" s="5">
         <v>0.9</v>
@@ -5906,16 +5862,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E74" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F74" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G74" s="5">
         <v>10.77</v>
@@ -5923,16 +5879,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="E75" t="s">
         <v>83</v>
       </c>
-      <c r="E75" t="s">
-        <v>87</v>
-      </c>
       <c r="F75" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G75" s="5">
         <v>7.8</v>
@@ -5940,16 +5896,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="E76" t="s">
+        <v>83</v>
+      </c>
+      <c r="F76" t="s">
         <v>84</v>
-      </c>
-      <c r="E76" t="s">
-        <v>87</v>
-      </c>
-      <c r="F76" t="s">
-        <v>88</v>
       </c>
       <c r="G76" s="5">
         <v>7.8</v>
@@ -5979,7 +5935,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -5988,7 +5944,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -6002,15 +5958,15 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -6021,15 +5977,15 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -6040,15 +5996,15 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -6077,13 +6033,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -6094,13 +6050,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -6111,13 +6067,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -6128,13 +6084,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -6145,13 +6101,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -6162,13 +6118,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -6179,13 +6135,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -6196,13 +6152,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -6213,13 +6169,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
         <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -6233,16 +6189,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -6253,16 +6209,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -6273,16 +6229,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -6293,16 +6249,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -6313,16 +6269,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
         <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -6333,10 +6289,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -6348,13 +6304,13 @@
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -6365,13 +6321,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
         <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -6382,13 +6338,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -6407,7 +6363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -6425,10 +6381,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -6445,10 +6401,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F2">
         <v>20</v>
@@ -6459,10 +6415,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F3">
         <v>70</v>
@@ -6473,10 +6429,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -6490,10 +6446,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -6507,10 +6463,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -6524,10 +6480,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -6541,10 +6497,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -6558,10 +6514,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -6575,10 +6531,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -6592,10 +6548,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -6609,10 +6565,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -6626,10 +6582,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" t="s">
         <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -6643,10 +6599,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -6660,10 +6616,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -6677,10 +6633,10 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -6694,10 +6650,10 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
         <v>115</v>
-      </c>
-      <c r="D19" t="s">
-        <v>119</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -6711,7 +6667,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -6727,7 +6683,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -6741,10 +6697,10 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -6758,10 +6714,10 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -6775,10 +6731,10 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -6792,10 +6748,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -6809,10 +6765,10 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -6826,10 +6782,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
         <v>115</v>
-      </c>
-      <c r="D31" t="s">
-        <v>119</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -6865,7 +6821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -6882,10 +6838,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -6899,10 +6855,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -6916,10 +6872,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -6933,10 +6889,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -6950,10 +6906,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -6967,10 +6923,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -6984,10 +6940,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -7001,10 +6957,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -7018,10 +6974,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -7035,10 +6991,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -7052,10 +7008,10 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -7069,10 +7025,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -7086,10 +7042,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -7103,10 +7059,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -7120,10 +7076,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -7137,10 +7093,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -7154,10 +7110,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -7171,10 +7127,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -7188,10 +7144,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -7205,10 +7161,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
@@ -7222,10 +7178,10 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -7239,10 +7195,10 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -7256,10 +7212,10 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
@@ -7273,10 +7229,10 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -7290,10 +7246,10 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -7307,10 +7263,10 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -7324,10 +7280,10 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -7341,10 +7297,10 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -7358,10 +7314,10 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -7375,10 +7331,10 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
@@ -7392,10 +7348,10 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -7409,10 +7365,10 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -7426,10 +7382,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -7443,10 +7399,10 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
@@ -7460,10 +7416,10 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
@@ -7477,10 +7433,10 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
@@ -7494,10 +7450,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
@@ -7511,10 +7467,10 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
@@ -7528,10 +7484,10 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
@@ -7545,10 +7501,10 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
@@ -7567,7 +7523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M17" activeCellId="1" sqref="A1:C1 M17"/>
     </sheetView>
   </sheetViews>
@@ -7585,7 +7541,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -7605,7 +7561,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>

</xml_diff>